<commit_message>
add image slider to card
</commit_message>
<xml_diff>
--- a/Kvota/wwwroot/ГОТОВЫЙ1111.xlsx
+++ b/Kvota/wwwroot/ГОТОВЫЙ1111.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="46">
   <si>
     <t xml:space="preserve">имя</t>
   </si>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Вилка PLS-3 (разъем PLS-40-G)</t>
   </si>
   <si>
-    <t xml:space="preserve">Бренд1</t>
+    <t xml:space="preserve">Бренд3</t>
   </si>
   <si>
     <t xml:space="preserve">Разьемы-Соединители</t>
@@ -64,6 +64,9 @@
     <t xml:space="preserve">Разьемы штыревые</t>
   </si>
   <si>
+    <t xml:space="preserve">jgjgjgjgjоппопопопопопопопопопопопопопа</t>
+  </si>
+  <si>
     <t xml:space="preserve">вилка ВН-10R C3510-10RPGB00 (разъем IDC-10MR)</t>
   </si>
   <si>
@@ -74,9 +77,6 @@
   </si>
   <si>
     <t xml:space="preserve">вилка ВН-26G (разъем ВН-26G)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Бренд3</t>
   </si>
   <si>
     <t xml:space="preserve">вилка ВН-50G (разъем ВН-50G)</t>
@@ -304,7 +304,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -387,8 +387,8 @@
   </sheetPr>
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -445,6 +445,9 @@
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>14</v>
+      </c>
       <c r="G2" s="3" t="n">
         <v>8.15232163080408</v>
       </c>
@@ -454,10 +457,10 @@
     </row>
     <row r="3" customFormat="false" ht="53.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -474,10 +477,10 @@
     </row>
     <row r="4" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -494,10 +497,10 @@
     </row>
     <row r="5" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -517,7 +520,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -537,7 +540,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -917,7 +920,7 @@
         <v>44</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G29" s="3" t="n">
         <v>605</v>

</xml_diff>